<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@49d20f5212f60581ff8177ebe458196da9b0ee07 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-My-core-goal.xlsx
+++ b/StructureDefinition-My-core-goal.xlsx
@@ -1265,17 +1265,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="28.609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="28.609375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="24.52734375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="24.52734375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="34.21875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="96.875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="83.0546875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1284,25 +1284,25 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="137.9609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="56.37109375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.859375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="118.27734375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="48.328125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="29.88671875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="30.0546875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="99.94921875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="25.765625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="85.6875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="31.65234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@9ec68cd033b552a1885c95da2e41d223eff1eb92 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-My-core-goal.xlsx
+++ b/StructureDefinition-My-core-goal.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="296">
   <si>
     <t>Property</t>
   </si>
@@ -642,6 +642,9 @@
   </si>
   <si>
     <t>Subject is optional to support annonymized reporting.</t>
+  </si>
+  <si>
+    <t>FOO</t>
   </si>
   <si>
     <t>PID-3-patient ID list</t>
@@ -3146,7 +3149,7 @@
         <v>76</v>
       </c>
       <c r="T17" t="s" s="2">
-        <v>76</v>
+        <v>202</v>
       </c>
       <c r="U17" t="s" s="2">
         <v>76</v>
@@ -3197,21 +3200,21 @@
         <v>99</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3234,17 +3237,17 @@
         <v>88</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>76</v>
@@ -3272,10 +3275,10 @@
         <v>174</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Z18" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AA18" t="s" s="2">
         <v>76</v>
@@ -3293,7 +3296,7 @@
         <v>76</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>77</v>
@@ -3314,15 +3317,15 @@
         <v>76</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3345,19 +3348,19 @@
         <v>76</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>76</v>
@@ -3406,7 +3409,7 @@
         <v>76</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>77</v>
@@ -3415,10 +3418,10 @@
         <v>78</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>76</v>
@@ -3432,10 +3435,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3458,13 +3461,13 @@
         <v>76</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -3515,7 +3518,7 @@
         <v>76</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>77</v>
@@ -3533,7 +3536,7 @@
         <v>76</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>76</v>
@@ -3541,10 +3544,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3573,7 +3576,7 @@
         <v>134</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="N21" t="s" s="2">
         <v>136</v>
@@ -3626,7 +3629,7 @@
         <v>76</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>77</v>
@@ -3644,7 +3647,7 @@
         <v>76</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>76</v>
@@ -3652,14 +3655,14 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
@@ -3681,10 +3684,10 @@
         <v>133</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N22" t="s" s="2">
         <v>136</v>
@@ -3739,7 +3742,7 @@
         <v>76</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>77</v>
@@ -3765,10 +3768,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -3794,10 +3797,10 @@
         <v>164</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -3827,10 +3830,10 @@
         <v>174</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>76</v>
@@ -3848,7 +3851,7 @@
         <v>76</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>77</v>
@@ -3857,7 +3860,7 @@
         <v>87</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>99</v>
@@ -3874,10 +3877,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -3900,16 +3903,16 @@
         <v>88</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -3938,7 +3941,7 @@
         <v>174</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>76</v>
@@ -3959,7 +3962,7 @@
         <v>76</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>77</v>
@@ -3968,7 +3971,7 @@
         <v>87</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>99</v>
@@ -3985,10 +3988,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4011,17 +4014,17 @@
         <v>88</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>76</v>
@@ -4070,7 +4073,7 @@
         <v>76</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>77</v>
@@ -4091,15 +4094,15 @@
         <v>76</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4122,16 +4125,16 @@
         <v>88</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
@@ -4181,7 +4184,7 @@
         <v>76</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>77</v>
@@ -4202,15 +4205,15 @@
         <v>76</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4233,16 +4236,16 @@
         <v>76</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
@@ -4292,7 +4295,7 @@
         <v>76</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>77</v>
@@ -4318,10 +4321,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4344,16 +4347,16 @@
         <v>88</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4403,7 +4406,7 @@
         <v>76</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>77</v>
@@ -4424,15 +4427,15 @@
         <v>76</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4455,17 +4458,17 @@
         <v>76</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>76</v>
@@ -4514,7 +4517,7 @@
         <v>76</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>77</v>
@@ -4532,18 +4535,18 @@
         <v>76</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4566,19 +4569,19 @@
         <v>76</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="O30" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="P30" t="s" s="2">
         <v>76</v>
@@ -4627,7 +4630,7 @@
         <v>76</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>77</v>
@@ -4642,10 +4645,10 @@
         <v>99</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>76</v>
@@ -4653,10 +4656,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -4682,16 +4685,16 @@
         <v>164</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>76</v>
@@ -4719,10 +4722,10 @@
         <v>174</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="Z31" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>76</v>
@@ -4740,7 +4743,7 @@
         <v>76</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>77</v>
@@ -4766,10 +4769,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -4792,19 +4795,19 @@
         <v>76</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O32" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>76</v>
@@ -4853,7 +4856,7 @@
         <v>76</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>77</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@8ff95042143bab90cdffc4c917ec24ed21524dd1 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-My-core-goal.xlsx
+++ b/StructureDefinition-My-core-goal.xlsx
@@ -616,7 +616,7 @@
     <t>Value set to describe the Goal</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/ValueSet/My-core-goal-description</t>
+    <t>http://loinc.org/vs/valid-hl7-attachment-requests</t>
   </si>
   <si>
     <t>GOL-3.2-goal ID.text</t>
@@ -1293,7 +1293,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="118.27734375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="48.328125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="39.17578125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>

</xml_diff>